<commit_message>
Added bulk upload api
</commit_message>
<xml_diff>
--- a/Bulk-customer-data.xlsx
+++ b/Bulk-customer-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KripaDev\Coding\wms-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2F04F4-5278-4292-8F3B-D394CE6B9F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE81F99-5E55-4E8D-BDA2-559C63BD48E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{429D1742-FD4C-4460-8FD3-34D09CFDC8DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>First Name</t>
   </si>
@@ -45,17 +45,53 @@
     <t>Mobile Number</t>
   </si>
   <si>
-    <t>Kripa</t>
-  </si>
-  <si>
     <t>Sharma</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>PINCODE</t>
+  </si>
+  <si>
+    <t>test101</t>
+  </si>
+  <si>
+    <t>test102</t>
+  </si>
+  <si>
+    <t>test103</t>
+  </si>
+  <si>
+    <t>test104</t>
+  </si>
+  <si>
+    <t>t101@gmail.com</t>
+  </si>
+  <si>
+    <t>t102@gmail.com</t>
+  </si>
+  <si>
+    <t>t103@gmail.com</t>
+  </si>
+  <si>
+    <t>t104@gmail.com</t>
+  </si>
+  <si>
+    <t>BSR</t>
+  </si>
+  <si>
+    <t>BLR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +103,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,14 +133,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F7473C-AC81-4276-93B0-D91A9C2C5F8B}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,9 +467,10 @@
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="17.109375" customWidth="1"/>
     <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,19 +480,104 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>784352652</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>203001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>784352653</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>203001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>784352654</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>201005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>784352655</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>201005</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{CCC7D857-B1B4-4E4D-A65E-98C797DEB469}"/>
+    <hyperlink ref="D3:D5" r:id="rId2" display="t101@gmail.com" xr:uid="{28CE2CA1-96A3-438C-81AA-5FBAB383E2C0}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{D432CF33-3D7C-4CFA-AD20-4BEAF864228A}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{790D1F97-D8F2-4DFD-9673-E923EF39DBAC}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{1FCF04F9-3CE9-4059-A225-CB1D7FDA1E0B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>